<commit_message>
Implement methods to create and print report and to allow user to input desired excel file
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 4/src/orders.xlsx
+++ b/Assignments/Assignment 4/src/orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherthompson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Work/PycharmProjects/3522_A01066418/Assignments/Assignment 4/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2615A5-2D4E-D84E-A9C0-4721B32DEC0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E51679-7DBD-8C4B-A22E-FD4E0D960CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19620" xr2:uid="{7FD0183C-8BAB-794C-881D-3EDFAD996962}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" xr2:uid="{7FD0183C-8BAB-794C-881D-3EDFAD996962}"/>
   </bookViews>
   <sheets>
     <sheet name="COMP 3522 A4" sheetId="1" r:id="rId1"/>
@@ -697,7 +697,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,7 +793,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -828,7 +828,7 @@
         <v>18</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>

</xml_diff>